<commit_message>
Project 1 code till Sep 25th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\012LivetechWS\HybridFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F879DF-5210-4BF3-9549-DA806E653722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B120EDA-3E7D-4BDF-AB1A-6D1CA4E10510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A176B97-7D08-43CF-852F-819A98689553}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
   <si>
     <t>TC- 101</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>reyaz456</t>
+  </si>
+  <si>
+    <t>TC-113</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>Hotel Creek</t>
+  </si>
+  <si>
+    <t>Check In Date</t>
+  </si>
+  <si>
+    <t>27/09/2024</t>
   </si>
 </sst>
 </file>
@@ -102,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A0C6E2-DAFD-4000-A884-2BAF155C94EF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,9 +451,11 @@
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -459,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -473,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -485,6 +509,52 @@
       </c>
       <c r="D5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>